<commit_message>
Added excel capability in Automation
</commit_message>
<xml_diff>
--- a/resource/mydata.xlsx
+++ b/resource/mydata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\AutomationPract\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98007923-C7DD-4EC8-9EF1-2BDC556BC634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28951D7D-D682-4DCF-9D61-3B0791A608BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5230AAE-5E9F-4430-A047-E4C3707ABEEC}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -48,17 +48,22 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>AdminSaurabTest@gmail.com</t>
+  </si>
+  <si>
+    <t>emailid</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,15 +409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3659CB6F-909F-43AB-850C-E37A5329E5C2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,10 +428,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -431,7 +445,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>